<commit_message>
Genereate random password and send email
</commit_message>
<xml_diff>
--- a/upload/template/employee/Bulk Upload Template.xlsx
+++ b/upload/template/employee/Bulk Upload Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Technologies" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="72">
   <si>
     <t xml:space="preserve">Sr. No</t>
   </si>
@@ -135,9 +135,6 @@
     <t xml:space="preserve">E0125</t>
   </si>
   <si>
-    <t xml:space="preserve">Ranjana Mishra</t>
-  </si>
-  <si>
     <t xml:space="preserve">ranjana@quadwave.com</t>
   </si>
   <si>
@@ -184,6 +181,39 @@
   </si>
   <si>
     <t xml:space="preserve">juhi@quadwave.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E0130</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mishra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mishranjana21@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E0131</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dmrunali613@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E0132</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vinit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dondapativinit@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E0133</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pratiksha </t>
+  </si>
+  <si>
+    <t xml:space="preserve">pratikshawa20@gmail.com</t>
   </si>
   <si>
     <t xml:space="preserve">Sr.No</t>
@@ -486,10 +516,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -572,7 +602,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="n">
         <v>2</v>
       </c>
@@ -604,7 +634,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="n">
         <v>3</v>
       </c>
@@ -668,16 +698,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="n">
         <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="6" t="s">
-        <v>37</v>
-      </c>
+      <c r="C6" s="6"/>
       <c r="D6" s="7" t="n">
         <v>44922</v>
       </c>
@@ -688,7 +716,7 @@
         <v>20</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H6" s="6" t="s">
         <v>22</v>
@@ -705,10 +733,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>39</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>40</v>
       </c>
       <c r="D7" s="7" t="n">
         <v>44923</v>
@@ -717,13 +745,13 @@
         <v>35952</v>
       </c>
       <c r="F7" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G7" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="H7" s="6" t="s">
         <v>42</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>43</v>
       </c>
       <c r="I7" s="9" t="n">
         <v>9823546721</v>
@@ -732,15 +760,15 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="n">
         <v>7</v>
       </c>
       <c r="B8" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>45</v>
       </c>
       <c r="D8" s="7" t="n">
         <v>44924</v>
@@ -752,10 +780,10 @@
         <v>26</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I8" s="9" t="n">
         <v>9052086452</v>
@@ -764,15 +792,15 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="n">
         <v>8</v>
       </c>
       <c r="B9" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>47</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>48</v>
       </c>
       <c r="D9" s="7" t="n">
         <v>44925</v>
@@ -781,13 +809,13 @@
         <v>35952</v>
       </c>
       <c r="F9" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="G9" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="G9" s="8" t="s">
-        <v>50</v>
-      </c>
       <c r="H9" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I9" s="9" t="n">
         <v>1209782345</v>
@@ -801,10 +829,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" s="0" t="s">
         <v>51</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>52</v>
       </c>
       <c r="D10" s="7" t="n">
         <v>44926</v>
@@ -813,10 +841,10 @@
         <v>35953</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H10" s="0" t="s">
         <v>22</v>
@@ -825,6 +853,134 @@
         <v>4123487659</v>
       </c>
       <c r="J10" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11" s="7" t="n">
+        <v>44918</v>
+      </c>
+      <c r="E11" s="7" t="n">
+        <v>35952</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I11" s="9" t="n">
+        <v>8723456712</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="5" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="7" t="n">
+        <v>44918</v>
+      </c>
+      <c r="E12" s="7" t="n">
+        <v>35952</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I12" s="9" t="n">
+        <v>9876452367</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" s="7" t="n">
+        <v>44918</v>
+      </c>
+      <c r="E13" s="7" t="n">
+        <v>35952</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="I13" s="9" t="n">
+        <v>1234543267</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="5" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D14" s="7" t="n">
+        <v>44918</v>
+      </c>
+      <c r="E14" s="7" t="n">
+        <v>35952</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I14" s="9" t="n">
+        <v>2345678990</v>
+      </c>
+      <c r="J14" s="6" t="s">
         <v>23</v>
       </c>
     </row>
@@ -860,7 +1016,7 @@
   </sheetPr>
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -873,10 +1029,10 @@
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -884,7 +1040,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -892,7 +1048,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -900,7 +1056,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -908,7 +1064,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -916,7 +1072,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -924,7 +1080,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix the bugs of bulk upload for role and technology
</commit_message>
<xml_diff>
--- a/upload/template/employee/Bulk Upload Template.xlsx
+++ b/upload/template/employee/Bulk Upload Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Technologies" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="54">
   <si>
     <t xml:space="preserve">Sr. No</t>
   </si>
@@ -90,7 +90,7 @@
     <t xml:space="preserve">Pune</t>
   </si>
   <si>
-    <t xml:space="preserve">E0122</t>
+    <t xml:space="preserve">E0123</t>
   </si>
   <si>
     <t xml:space="preserve">Mrunali Desai</t>
@@ -102,9 +102,6 @@
     <t xml:space="preserve">mrunali@quadwave.com</t>
   </si>
   <si>
-    <t xml:space="preserve">E0123</t>
-  </si>
-  <si>
     <t xml:space="preserve">Suraksha Nigade</t>
   </si>
   <si>
@@ -115,9 +112,6 @@
   </si>
   <si>
     <t xml:space="preserve">E0124</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pratiksha Sanam</t>
   </si>
   <si>
     <t xml:space="preserve">.NET Developer</t>
@@ -382,8 +376,8 @@
   </sheetPr>
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -467,8 +461,8 @@
   </sheetPr>
   <dimension ref="A1:J1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="1" sqref="B7 B9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -588,10 +582,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>26</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>27</v>
       </c>
       <c r="D4" s="7" t="n">
         <v>44920</v>
@@ -600,10 +594,10 @@
         <v>35952</v>
       </c>
       <c r="F4" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" s="8" t="s">
         <v>28</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>29</v>
       </c>
       <c r="H4" s="6" t="s">
         <v>20</v>
@@ -615,16 +609,14 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="n">
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>31</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="C5" s="6"/>
       <c r="D5" s="7" t="n">
         <v>44921</v>
       </c>
@@ -632,10 +624,10 @@
         <v>35952</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H5" s="6" t="s">
         <v>20</v>
@@ -652,10 +644,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D6" s="7" t="n">
         <v>44922</v>
@@ -667,7 +659,7 @@
         <v>18</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H6" s="6" t="s">
         <v>20</v>
@@ -684,10 +676,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D7" s="7" t="n">
         <v>44923</v>
@@ -696,13 +688,13 @@
         <v>35952</v>
       </c>
       <c r="F7" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="H7" s="6" t="s">
         <v>39</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>41</v>
       </c>
       <c r="I7" s="9" t="n">
         <v>9823546721</v>
@@ -716,10 +708,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D8" s="7" t="n">
         <v>44924</v>
@@ -731,10 +723,10 @@
         <v>24</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I8" s="9" t="n">
         <v>9052086452</v>
@@ -748,10 +740,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D9" s="7" t="n">
         <v>44925</v>
@@ -760,13 +752,13 @@
         <v>35952</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I9" s="9" t="n">
         <v>1209782345</v>
@@ -780,10 +772,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D10" s="7" t="n">
         <v>44926</v>
@@ -792,10 +784,10 @@
         <v>35953</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H10" s="0" t="s">
         <v>20</v>
@@ -844,7 +836,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H14" activeCellId="1" sqref="B7 H14"/>
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -856,10 +848,10 @@
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -867,7 +859,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -881,7 +873,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -889,7 +881,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -903,7 +895,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Resolve add employee issue
</commit_message>
<xml_diff>
--- a/upload/template/employee/Bulk Upload Template.xlsx
+++ b/upload/template/employee/Bulk Upload Template.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="44">
   <si>
     <t xml:space="preserve">Sr. No</t>
   </si>
@@ -123,13 +123,22 @@
     <t xml:space="preserve">p11@gmail.com</t>
   </si>
   <si>
-    <t xml:space="preserve">E0112</t>
-  </si>
-  <si>
-    <t xml:space="preserve">p12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">p12@gmail.com</t>
+    <t xml:space="preserve">E0114</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p14@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E0115</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p15@gmail.com</t>
   </si>
   <si>
     <t xml:space="preserve">Sr.No</t>
@@ -428,10 +437,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -657,6 +666,41 @@
         <v>22</v>
       </c>
       <c r="K6" s="3" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="9" t="n">
+        <v>44922</v>
+      </c>
+      <c r="E7" s="9" t="n">
+        <v>35954</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="I7" s="11" t="n">
+        <v>1234543268</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="K7" s="3" t="n">
         <v>2</v>
       </c>
     </row>
@@ -697,10 +741,10 @@
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -708,7 +752,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -724,7 +768,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -732,7 +776,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -748,7 +792,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Create mapping for user and current role and created mobile and location is optional while bulk upload it will not show remark and status failed
</commit_message>
<xml_diff>
--- a/upload/template/employee/Bulk Upload Template.xlsx
+++ b/upload/template/employee/Bulk Upload Template.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="59">
   <si>
     <t xml:space="preserve">Sr. No</t>
   </si>
@@ -139,6 +139,51 @@
   </si>
   <si>
     <t xml:space="preserve">p15@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E0119</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p19@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E0120</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p20@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E0121</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p21@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E0122</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p22@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E0123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p23@gmail.com</t>
   </si>
   <si>
     <t xml:space="preserve">Sr.No</t>
@@ -437,10 +482,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G12" activeCellId="0" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -702,6 +747,175 @@
       </c>
       <c r="K7" s="3" t="n">
         <v>2</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="9" t="n">
+        <v>44922</v>
+      </c>
+      <c r="E8" s="9" t="n">
+        <v>35967</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="I8" s="11" t="n">
+        <v>1234543268</v>
+      </c>
+      <c r="J8" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="K8" s="3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" s="9" t="n">
+        <v>44922</v>
+      </c>
+      <c r="E9" s="9" t="n">
+        <v>35959</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="I9" s="11" t="n">
+        <v>1234543268</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="K9" s="3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" s="9" t="n">
+        <v>44922</v>
+      </c>
+      <c r="E10" s="9" t="n">
+        <v>35964</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="I10" s="11" t="n">
+        <v>1234543268</v>
+      </c>
+      <c r="J10" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="K10" s="3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="9" t="n">
+        <v>44922</v>
+      </c>
+      <c r="E11" s="9" t="n">
+        <v>35964</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="I11" s="11"/>
+      <c r="J11" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="K11" s="3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" s="9" t="n">
+        <v>44922</v>
+      </c>
+      <c r="E12" s="9" t="n">
+        <v>35964</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="I12" s="11"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="3" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -741,10 +955,10 @@
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -752,7 +966,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -768,7 +982,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -776,7 +990,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -792,7 +1006,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Set remark for update existing employee data and add logger.
</commit_message>
<xml_diff>
--- a/upload/template/employee/Bulk Upload Template.xlsx
+++ b/upload/template/employee/Bulk Upload Template.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="59">
   <si>
     <t xml:space="preserve">Sr. No</t>
   </si>
@@ -484,8 +484,8 @@
   </sheetPr>
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G12" activeCellId="0" sqref="G12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -661,7 +661,7 @@
         <v>35953</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="G5" s="10" t="s">
         <v>32</v>
@@ -903,9 +903,7 @@
       <c r="E12" s="9" t="n">
         <v>35964</v>
       </c>
-      <c r="F12" s="8" t="s">
-        <v>19</v>
-      </c>
+      <c r="F12" s="8"/>
       <c r="G12" s="10" t="s">
         <v>53</v>
       </c>

</xml_diff>